<commit_message>
Pipeline complet version 1
</commit_message>
<xml_diff>
--- a/assets/00_master/master_template.xlsx
+++ b/assets/00_master/master_template.xlsx
@@ -5,21 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosch\Bureau\KAIVAA\kaivaa-builder\assets\00_excel_master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosch\Bureau\KAIVAA\kaivaa-builder\assets\00_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95371C05-481A-4856-8D67-4B1E6D085684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6B06C7-8BC6-4380-8BCC-17DA3ED5F89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1FFF5854-B54B-4C80-B65C-C43C5EF7384C}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{1FFF5854-B54B-4C80-B65C-C43C5EF7384C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data -&gt;" sheetId="52" r:id="rId1"/>
     <sheet name="Settings -&gt;" sheetId="51" r:id="rId2"/>
-    <sheet name="Balises" sheetId="9" r:id="rId3"/>
-    <sheet name="Boucles" sheetId="5" r:id="rId4"/>
-    <sheet name="Liste" sheetId="49" r:id="rId5"/>
-    <sheet name="Tables" sheetId="48" r:id="rId6"/>
-    <sheet name="Analyses -&gt;" sheetId="50" r:id="rId7"/>
+    <sheet name="Paramètrage" sheetId="53" r:id="rId3"/>
+    <sheet name="Balises" sheetId="9" r:id="rId4"/>
+    <sheet name="Boucles" sheetId="5" r:id="rId5"/>
+    <sheet name="Liste" sheetId="49" r:id="rId6"/>
+    <sheet name="Tables" sheetId="48" r:id="rId7"/>
+    <sheet name="Analyses -&gt;" sheetId="50" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Balise</t>
   </si>
@@ -257,6 +258,51 @@
       </rPr>
       <t xml:space="preserve"> Tables</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Paramétrage</t>
+    </r>
+  </si>
+  <si>
+    <t>Centralisez tous les paramètres devant être saisis par l'utilisateur pour faire fonctionner le modèle</t>
   </si>
 </sst>
 </file>
@@ -326,12 +372,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF6D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -366,6 +406,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -388,37 +434,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,20 +488,18 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
           <color theme="1"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -484,15 +527,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
           <color theme="1"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -514,20 +555,18 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFF6D9"/>
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
           <color theme="1"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -708,10 +747,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D6EACE5-26DB-4F7F-9487-26DB7B53498F}" name="Loop" displayName="Loop" ref="C6:F7" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="C6:F7" xr:uid="{9D6EACE5-26DB-4F7F-9487-26DB7B53498F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{57A92AE8-0D79-4270-A771-98B4928EEDE3}" name="ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{0153B2F4-CF5A-40D7-B52A-8736C7DFED4F}" name="Itération" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{57A92AE8-0D79-4270-A771-98B4928EEDE3}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{0153B2F4-CF5A-40D7-B52A-8736C7DFED4F}" name="Itération" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{C2F670A5-B30E-4FDD-A0FC-6BAE9E92844D}" name="Nombre de tests" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{5E26AB54-DDBA-4A1A-B5B5-6BF98CC52480}" name="Résultat" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{5E26AB54-DDBA-4A1A-B5B5-6BF98CC52480}" name="Résultat" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -951,7 +990,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -971,7 +1010,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -979,69 +1018,86 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CABEDE1-7C2C-4CA0-9D01-11D3699B5D3D}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.749992370372631"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:3" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBD2C17-1A96-495A-A6EE-E3BE98E820C5}">
   <sheetPr>
     <tabColor theme="1" tint="0.749992370372631"/>
   </sheetPr>
   <dimension ref="B1:F9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
     <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="66.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="6"/>
+    <col min="7" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="8"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="8"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1057,9 +1113,9 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1071,7 +1127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733D94AE-0F52-4E43-9936-FBC5DD02B773}">
   <sheetPr>
     <tabColor theme="1" tint="0.749992370372631"/>
@@ -1079,39 +1135,39 @@
   <dimension ref="B1:G7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="6"/>
+    <col min="8" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C5" s="12"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C6" s="2" t="s">
@@ -1129,8 +1185,8 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="3"/>
     </row>
   </sheetData>
@@ -1141,12 +1197,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4DEE71-DE17-4D4C-BDEA-03D77B89170F}">
   <sheetPr>
     <tabColor theme="1" tint="0.749992370372631"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -1154,39 +1210,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:3" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="1" spans="3:3" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C8" s="12"/>
+      <c r="C8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D026D111-3B59-41A1-BB6B-B78335779B29}">
   <sheetPr>
     <tabColor theme="1" tint="0.749992370372631"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -1194,27 +1249,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:3" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="1" spans="3:3" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C8" s="12"/>
+      <c r="C8" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1222,7 +1276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB59BF7C-EBB7-4520-B112-23863CFF38C4}">
   <sheetPr>
     <tabColor theme="1" tint="9.9978637043366805E-2"/>
@@ -1235,7 +1289,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>